<commit_message>
Tested decision tree with different criterion, updated result
</commit_message>
<xml_diff>
--- a/classifiers/github_labels/decision_tree/report.xlsx
+++ b/classifiers/github_labels/decision_tree/report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17668"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="13">
   <si>
     <t>Decision Tree</t>
   </si>
@@ -49,13 +49,22 @@
   </si>
   <si>
     <t>90 by 5</t>
+  </si>
+  <si>
+    <t>Criterion</t>
+  </si>
+  <si>
+    <t>gini</t>
+  </si>
+  <si>
+    <t>entropy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,16 +102,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,8 +126,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -149,13 +156,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
@@ -166,17 +185,21 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="20% - Accent5" xfId="3" builtinId="46"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="2" builtinId="10"/>
@@ -457,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,9 +494,10 @@
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,8 +516,11 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>2</v>
       </c>
@@ -503,14 +530,17 @@
       <c r="D2">
         <v>0.223</v>
       </c>
-      <c r="E2" s="7">
+      <c r="E2" s="9">
         <v>71.900000000000006</v>
       </c>
       <c r="F2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>50</v>
       </c>
@@ -520,14 +550,17 @@
       <c r="D3">
         <v>0.22</v>
       </c>
-      <c r="E3" s="7">
+      <c r="E3" s="9">
         <v>73.069999999999993</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>100</v>
       </c>
@@ -537,14 +570,17 @@
       <c r="D4">
         <v>0.23</v>
       </c>
-      <c r="E4" s="7">
+      <c r="E4" s="9">
         <v>73.94</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>1000</v>
       </c>
@@ -554,14 +590,17 @@
       <c r="D5">
         <v>0.2</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="9">
         <v>69.400000000000006</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3">
         <v>500</v>
@@ -572,14 +611,17 @@
       <c r="D6" s="3">
         <v>0.23300000000000001</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="10">
         <v>74.319999999999993</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>250</v>
       </c>
@@ -589,14 +631,17 @@
       <c r="D7">
         <v>0.2</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="9">
         <v>73.569999999999993</v>
       </c>
       <c r="F7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3">
         <v>300</v>
@@ -607,14 +652,17 @@
       <c r="D8" s="3">
         <v>0.26</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="10">
         <v>74.12</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4">
         <v>300</v>
@@ -625,14 +673,17 @@
       <c r="D9" s="4">
         <v>0.21</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="11">
         <v>74.95</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4">
         <v>300</v>
@@ -643,47 +694,202 @@
       <c r="D10" s="4">
         <v>0.23</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="11">
         <v>76.3</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4">
         <v>300</v>
       </c>
       <c r="C11" s="4">
+        <v>265</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="E11" s="11">
         <v>77.52</v>
-      </c>
-      <c r="D11" s="4">
-        <v>265</v>
-      </c>
-      <c r="E11" s="6">
-        <v>0.2</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4">
         <v>500</v>
       </c>
       <c r="C12" s="4">
+        <v>266</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.23</v>
+      </c>
+      <c r="E12" s="11">
         <v>77.47</v>
-      </c>
-      <c r="D12" s="4">
-        <v>266</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0.23</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>9</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="E13" s="9">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>50</v>
+      </c>
+      <c r="E14" s="9">
+        <v>73.05</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>100</v>
+      </c>
+      <c r="E15" s="9">
+        <v>73.430000000000007</v>
+      </c>
+      <c r="F15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1000</v>
+      </c>
+      <c r="E16" s="9">
+        <v>66.03</v>
+      </c>
+      <c r="F16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>500</v>
+      </c>
+      <c r="E17" s="9">
+        <v>73.5</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>250</v>
+      </c>
+      <c r="E18" s="9">
+        <v>73.5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>300</v>
+      </c>
+      <c r="E19" s="9">
+        <v>72.92</v>
+      </c>
+      <c r="F19" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>250</v>
+      </c>
+      <c r="E20" s="9"/>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>250</v>
+      </c>
+      <c r="E21" s="9"/>
+      <c r="F21" t="s">
+        <v>8</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>250</v>
+      </c>
+      <c r="E22" s="9"/>
+      <c r="F22" t="s">
+        <v>9</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>250</v>
+      </c>
+      <c r="E23" s="9"/>
+      <c r="F23" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added classifiers - knn, randomforest & adaboost (ensemble)
got good results with randomForest
</commit_message>
<xml_diff>
--- a/classifiers/github_labels/decision_tree/report.xlsx
+++ b/classifiers/github_labels/decision_tree/report.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="15">
   <si>
     <t>Decision Tree</t>
   </si>
@@ -58,13 +58,19 @@
   </si>
   <si>
     <t>entropy</t>
+  </si>
+  <si>
+    <t>~0.5</t>
+  </si>
+  <si>
+    <t>~0.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,8 +108,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,6 +142,12 @@
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -174,7 +192,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="2" applyFont="1" applyAlignment="1">
@@ -186,8 +204,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -195,6 +217,19 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -483,7 +518,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection sqref="A1:G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,374 +556,449 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2">
+      <c r="B2" s="8">
         <v>2</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="8">
         <v>0.53</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="8">
         <v>0.223</v>
       </c>
       <c r="E2" s="9">
         <v>71.900000000000006</v>
       </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3">
+      <c r="B3" s="8">
         <v>50</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="8">
         <v>0.53</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="8">
         <v>0.22</v>
       </c>
       <c r="E3" s="9">
         <v>73.069999999999993</v>
       </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" s="7" t="s">
+      <c r="F3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4">
+      <c r="B4" s="8">
         <v>100</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="8">
         <v>0.46</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="8">
         <v>0.23</v>
       </c>
       <c r="E4" s="9">
         <v>73.94</v>
       </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="7" t="s">
+      <c r="F4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5">
+      <c r="B5" s="8">
         <v>1000</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="8">
         <v>0.08</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="8">
         <v>0.2</v>
       </c>
       <c r="E5" s="9">
         <v>69.400000000000006</v>
       </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="7" t="s">
+      <c r="F5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
-      <c r="B6" s="3">
+      <c r="B6" s="13">
         <v>500</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="13">
         <v>0.3</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="13">
         <v>0.23300000000000001</v>
       </c>
       <c r="E6" s="10">
         <v>74.319999999999993</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="7" t="s">
+      <c r="F6" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7">
+      <c r="B7" s="8">
         <v>250</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
         <v>0.47</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
         <v>0.2</v>
       </c>
       <c r="E7" s="9">
         <v>73.569999999999993</v>
       </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="7" t="s">
+      <c r="F7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="3">
+      <c r="B8" s="13">
         <v>300</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="13">
         <v>0.4</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="13">
         <v>0.26</v>
       </c>
       <c r="E8" s="10">
         <v>74.12</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="7" t="s">
+      <c r="F8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="4">
+      <c r="B9" s="7">
         <v>300</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="7">
         <v>2.1</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="7">
         <v>0.21</v>
       </c>
       <c r="E9" s="11">
         <v>74.95</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="4">
+      <c r="B10" s="7">
         <v>300</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="7">
         <v>71</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="7">
         <v>0.23</v>
       </c>
       <c r="E10" s="11">
         <v>76.3</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4">
+      <c r="A11" s="15"/>
+      <c r="B11" s="16">
         <v>300</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="16">
         <v>265</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="16">
         <v>0.23</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="16">
         <v>77.52</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="F11" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="4">
+      <c r="B12" s="7">
         <v>500</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="7">
         <v>266</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="7">
         <v>0.23</v>
       </c>
       <c r="E12" s="11">
         <v>77.47</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="7" t="s">
+      <c r="G12" s="12" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13">
+      <c r="B13" s="8">
         <v>2</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="E13" s="9">
         <v>71.599999999999994</v>
       </c>
-      <c r="F13" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="8" t="s">
+      <c r="F13" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14">
+      <c r="B14" s="8">
         <v>50</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="E14" s="9">
         <v>73.05</v>
       </c>
-      <c r="F14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G14" s="8" t="s">
+      <c r="F14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15">
+      <c r="B15" s="8">
         <v>100</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="E15" s="9">
         <v>73.430000000000007</v>
       </c>
-      <c r="F15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" s="8" t="s">
+      <c r="F15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16">
+      <c r="B16" s="8">
         <v>1000</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="E16" s="9">
         <v>66.03</v>
       </c>
-      <c r="F16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G16" s="8" t="s">
+      <c r="F16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
         <v>500</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="E17" s="9">
         <v>73.5</v>
       </c>
-      <c r="F17" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="8" t="s">
+      <c r="F17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="8">
         <v>250</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="E18" s="9">
         <v>73.5</v>
       </c>
-      <c r="F18" t="s">
-        <v>6</v>
-      </c>
-      <c r="G18" s="8" t="s">
+      <c r="F18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G18" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="8">
         <v>300</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>14</v>
       </c>
       <c r="E19" s="9">
         <v>72.92</v>
       </c>
-      <c r="F19" t="s">
-        <v>6</v>
-      </c>
-      <c r="G19" s="8" t="s">
+      <c r="F19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="8">
         <v>250</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" t="s">
+      <c r="C20" s="8">
+        <v>1.7</v>
+      </c>
+      <c r="D20" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="E20" s="9">
+        <v>75.290000000000006</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="3"/>
+      <c r="B21" s="13">
         <v>250</v>
       </c>
-      <c r="E21" s="9"/>
-      <c r="F21" t="s">
+      <c r="C21" s="13">
+        <v>61</v>
+      </c>
+      <c r="D21" s="13">
+        <v>0.27</v>
+      </c>
+      <c r="E21" s="13">
+        <v>76.3</v>
+      </c>
+      <c r="F21" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="8">
         <v>250</v>
       </c>
-      <c r="E22" s="9"/>
-      <c r="F22" t="s">
+      <c r="C22" s="8">
+        <v>206</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.27</v>
+      </c>
+      <c r="E22" s="9">
+        <v>77</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="14" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>250</v>
-      </c>
-      <c r="E23" s="9"/>
-      <c r="F23" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="8">
+        <v>500</v>
+      </c>
+      <c r="C23" s="8">
+        <v>204</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="E23" s="9">
+        <v>77.489999999999995</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="14" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>